<commit_message>
Add TC7-8-9-10-11-12 by Gilana and change Data Dictionary.docx
</commit_message>
<xml_diff>
--- a/DOCS/Test Cases/EditCrisis.xlsx
+++ b/DOCS/Test Cases/EditCrisis.xlsx
@@ -393,6 +393,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -408,8 +410,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -707,7 +707,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -776,7 +776,7 @@
       <c r="I2" s="7"/>
     </row>
     <row r="3" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="13" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="11" t="s">
@@ -792,7 +792,7 @@
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
     </row>
-    <row r="4" spans="1:10" ht="16.5" customHeight="1">
+    <row r="4" spans="1:10" ht="36" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>62</v>
       </c>
@@ -805,7 +805,7 @@
       <c r="D4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="11" t="s">
         <v>22</v>
       </c>
       <c r="F4" s="7"/>
@@ -813,7 +813,7 @@
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" ht="36" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>54</v>
       </c>
@@ -1062,7 +1062,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1082,43 +1082,43 @@
       <c r="A1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
       <c r="I1" s="8"/>
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="15" t="s">
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="17" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
       <c r="C3" s="9" t="s">
         <v>9</v>
       </c>
@@ -1135,7 +1135,7 @@
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
-      <c r="K3" s="16"/>
+      <c r="K3" s="18"/>
     </row>
     <row r="4" spans="1:11" ht="24.75" customHeight="1" thickTop="1">
       <c r="A4" s="8" t="s">
@@ -1241,7 +1241,7 @@
       <c r="A8" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="14" t="s">
         <v>50</v>
       </c>
       <c r="C8" s="8" t="s">

</xml_diff>